<commit_message>
Update to measure to map space_use to cbecs values
</commit_message>
<xml_diff>
--- a/spreadsheet/urban-spreadsheet.xlsx
+++ b/spreadsheet/urban-spreadsheet.xlsx
@@ -2283,9 +2283,6 @@
     <t>discrete</t>
   </si>
   <si>
-    <t>[0.2,0.2,0.2,0.1,0.1,0.1,0.1]</t>
-  </si>
-  <si>
     <t>Directory</t>
   </si>
   <si>
@@ -2295,16 +2292,19 @@
     <t>../urban_geometry_creation/tests</t>
   </si>
   <si>
-    <t>['142484','116245','142872','43254','1459','134032','143122']</t>
-  </si>
-  <si>
     <t>142484'</t>
   </si>
   <si>
-    <t>|'142484','116245','142872','43254','1459','134032','143122'|</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ../../../lib/city_data/city.json</t>
+  </si>
+  <si>
+    <t>|'142484','116245','142872','43254','1459','134032','143122','15204','155513','181948','142238','191582','185054','208359','113178','192702','236371','190013','6434','231850','128469','172662','222162','122347','158690','202694','56659','85635','3571','83186','227340','41962','217309','52660','161648','184642','3847','2373','62625','65373','58283','58911','237783','79514','110389','144568','5955','78754','96419','83574','223270','148046','191859','33879','52936','106804','221612','61663','207542','213989','49369','116055','151927','8514','100535','187338','207180','50936','11886','20763','230376','134949','151680','152016','164646','206572','178897','181797','183160','206869','187675','200594','222412','223723','233024','234608','235990','240241','203425','186746','215740','227893','230795','147716','150821','151683','155087','173389','208781','221871','236646','134575','138298','141692','146223','147538','148715','154723','155770','159371','166226','166447','185614','190700','200435','203431','209303','211686','225506','226857','231874','236181','134829','153445','188330','195998','215567','236722','240378','136118','144038','145786','156369','160789','166893','177498','184217','197688','212943','223606','224837','225080','228898','229908','234747','236146','236944','139179','140483','141333','141742','149927','150157','153100','157664','160763','164828','165203','166177','167379','169768','170121','170176','171097','172136','172760','174951','176543','188603','188635','192839','194021','194266','196939','199268','207526','207791','209874','210350','216983','219655','221577','225998','231823','233786','139210','139560','140971','148938','153385','156024','156566','157189','161540','162805','165776','181190','183554','184555','185691','187767','192580','196291','200692','203271','205426','209161','212361','212521','214551','220751','221103','222785','226178','234948','236366','238464','140303','155940','171027','184033','193357','206646','228561','240057','158140','159829','168276','181627','181985','194704','199802','200515','214462','220549','224670','231114','231559','238379','239180','139056','146495','160004','163839','170485','174902','176024','181799','188941','190575','192751','195570','212682','215390','222246','227246','232402','233696','238260','238366','138674','140217','149213','151733','155395','156878','157846','182991','197481','200860','204224','212394','215129','151466','157857','205201','208419','222958','224064','238013','142841','145861','145877','146423','165161','166962','171677','197554','199848','218849','219161','221310','234670','235539','239758','136089','138309','139280','139552','139972','140112','141291','145092','146832','147765','148030','149426','151459','151615','153585','154644','155425','156031','162031','158373','161939','163262','164664','168617','169885','169922','171070','173586','177972','178711','179427','179543','181848','183383','186074','186323','186484','186645','188930','189510','194658','197850','198151','204452','208462','210041','210801','211161','213948','214599','217006','220057','222119','229206','229762','236497','237377','240264','139906','142689','144492','161710','171251','173347','182732','199171','199748','218496','157559','161139','162145','175894','177668','179093','191030','211557','217141','218850','140479','152927','154431','154464','159986','179970','179999','184576','180201','187575','189920','190567','192647','207120','208849','212153','214562','218163','229721','229883','230166','233318','235390','135669','136042','146188','146794','150655','155019','159866','160735','164404','165424','172541','186414','176530','178186','181487','185242','190676','193814','196736','206032','212641','224220','224416','225635','233901','234701','237931','138231','141323','144648','145555','150780','150899','152839','156034','156206','157204','163155','164382','164577','166037','167180','171781','172656','175940','176083','176527','177893','179370','179380','180506','180928','181312','186261','186821','188752','188829','192028','192253','195430','196757','197324','204858','202564','203048','209777','209943','211983','215123','215882','217903','219176','227481','232103','234356','239047','144314','152718','161890','173232','184010','185603','189087','192262','195632','202699','223098','223836','224922','229421','140000','140062','168535','175315','179702','193716','211405','226429','212193','229689','156794','159799','163819','179634','181429','190947','205996','211049','224660','134586','140179','140897','148743','148792','153916','155447','161638','161681','163049','163218','186378','169820','177857','178398','182872','183800','188456','191281','191863','194747','199020','201060','205442','210315','214715','217037','218199','228236','229366','230278','230745','238378','238645','141358','141807','146429','151549','163349','159431','163012','176825','178193','189427','189930','191574','194472','196651','199478','205863','225950','231182','146349','161436','187104','191021','191734','194086','197836','203209','230430','136919','147914','150225','151174','151776','166433','170224','177521','185308','192052','200711','206227','210308','222863','222913','231145','236127','137197','140158','146957','148680','158508','167413','181146','188059','195832','215406','219282','221742','228771','230227','233235','137687','139905','148683','153540','154931','160185','161507','168943','175576','190299','194794','211649','213228','218327','227520','137733','143531','145229','152035','156082','162358','162560','166563','167482','174906','177785','179581','181727','184831','187591','188181','192875','197918','203955','205171','206049','211102','211511','140460','182042','185846','186059','194978','202325','207738','210823','213539','224910','143750','146664','157155','171037','185610','214994','222640','236462','135958','145554','152220','154793','155394','157781','173632','179192','190668','186750','191225','206920','218691','219325','221114','135888','137520','140523','142060','144519','145787','146424','147199','147684','154270','160406','161101','161838','163303','163875','164094','164561','166429','168479','168736','169732','172313','172383','175207','176225','178036','182775','186511','187648','188736','190841','194156','195367','195774','204083','210774','212113','214198','216378','218821','220433','232024','232440','235333','236582','239376','200511','200703','216368','216854','220985','221684','221834','221849','222135','223137','223721','224158','224504','226166','226297','226695','229251','230716','230761','234635','234895','235308','236196','237124','237960','238930','239976','240032','122105','168573','96922','144185','151931','156986','190213','217362','164013','104780','121861','167901','184630','124937','185146','193248','195079','77300','80971','86658','131929','204467','143637','203758','81361','106807','80313','131985','159184','212516','219061','143680','199109','200379','210667','213357','88336','90589','160050','187722','190416','196196','216274','108357','158067','191814','209748','218028','168409','88808','91652','107419','120394','130934','176535','186299','215284','72338','150378','155290','156516','157947','216010','219839','96387','103082','120734','122770','146527','147644','184966','107876','175298','184668','149130','150004','156304','174164','189171','84614','88533','90706','156563','179208','199464','80947','84283','85985','96257','101054','108605','122529','133615','137288','152785','169737','172060','218831','219358','83489','92916','108429','117211','119645','150610','149445','170454','184703','189645','190838','191674','214057','92414','115798','119426','128986','140277','154095','155957','160911','181632','126037','142972','305','557','784','3098','3672','4208','6537','7626','8122','9776','13779','16415','17391','17442','17741','18019','18138','20033','22734','23111','25358','26767','27364','27864','29168','30409','34851','35629','40383','37821','37934','38939','41644','42197','42305','42734','43507','43919','44444','44863','47006','47204','48052','59307','50573','53776','57248','58083','58533','62498','64663','65211','65916','66016','66723','67740','70467','73642','77256','78947','78958','79333','80104','80443','80717','81835','82425','82968','84578','87717','91015','91765','93806','96354','99101','99674','99978','103749','103853','104550','104801','105053','105736','105868','110303','110562','111378','111785','114642','117175','118705','123784','127336','127500','128766','129848','132134','132751','132950','133166','133776','131234','3671','4081','135435','12530','14875','25798','27308','30244','36571','41743','43437','44422','50607','55895','60525','66798','68600','68660','80402','82849','84693','92321','96066','107805','113252','116607','124001','130014','133034','132020','133819','1614','9787','15251','16859','18125','18253','21029','22044','24430','25821','30558','35912','39172','43686','44759','48274','48348','48952','49643','52210','55580','56230','56407','57930','57995','63830','65413','138646','71351','77608','102025','83878','84727','85039','89242','90596','91378','93895','94043','100388','101217','105518','106584','108694','111679','115046','114720','115805','118622','118763','119139','124080','128823','131551','132161','132761','132835','968','2145','2916','3901','7554','8131','8405','8875','9938','11008','11260','11633','14409','23443','27408','28907','29640','37909','38528','40120','60775','41112','42345','43161','44010','45630','46261','48335','54169','56205','57845','62892','65927','71052','72573','72609','72949','74596','74997','76347','77748','77875','78079','78374','79904','80019','80515','80904','81473','84188','102028','85108','92610','96690','98837','102417','103518','106075','106994','107133','107743','108418','109053','111513','114441','152173','120001','120466','124740','127774','129389','131553','133568','142275','128616','132155','124431','1835','4852','5970','5985','6412','6955','7065','7703','8979','9049','9917','10941','11426','13336','15743','15897','16700','17972','19474','21410','22635','23082','27277','29120','30449','31299','36733','37519','37960','38880','39273','43509','46157','46514','46973','50361','51850','53952','54531','57203','58449','62391','62627','62868','63596','138384','65272','67241','68865','69075','72535','73049','74789','75400','77048','79462','81655','86241','88606','88789','89145','89600','92602','94657','94900','95113','102086','95695','96505','100305','100408','100617','100621','100751','103105','105168','105373','105472','106890','110314','110661','111108','111294','112819','113515','117619','119304','120316','120521','120528','120659','124907','126403','129765','131946','132840','153878','5','803','2639','5453','5594','129144','8608','8891','11318','12098','12783','17960','18400','18679','20839','23247','23479','23920','25659','26382','28634','31791','33691','36559','37647','37686','38127','38824','38946','40172','43126','44441','45829','46984','47544','49109','49486','52170','128455','57399','58303','63100','63763','64448','64981','65895','128047','66289','67269','67319','69236','70023','71428','71681','74427','75660','75870','76389','77814','78152','81308','80554','127991','82858','83539','84011','88645','89138','89758','92226','94088','95964','97567','98652','100307','101113','102703','104239','105170','106108','106842','106907','109530','110458','114806','114884','114941','115031','116830','118122','120000','121285','9024','128624','129618','130084','132992','2029','2594','3371','6931','7325','8446','8837','10917','12757','13544','14020','17641','17956','19344','21647','22075','39354','24708','24967','29565','29572','30608','31214','32653','33914','34278','36147','38435','41529','44877','47239','48848','48908','51292','52433','52552','52699','52792','54130','56588','57681','58385','58941','59934','127472','60452','127483','65780','66892','67721','69590','69747','69880','70898','72508','74337','78317','79008','81699','82051','82348','83068','84196','86674','89038','90018','91299','92325','125673','93518','125382','98274','125485','99009','101785','102137','103741','104396','105700','108474','110143','110357','111635','111934','114266','114681','114932','115534','115558','115652','117848','118484','119292','119814','120456','120690','120792','120862','122837','135325','127676','130746','131123','128759','147482','410','5228','5975','6468','8136','13556','16203','20203','20467','21150','21907','22013','26278','27384','28663','30270','31941','32840','34162','34185','36119','36564','37307','39104','40441','40582','40730','42225','43182','165199','44991','45563','47205','47802','47968','48521','49230','50162','50277','50444','51280','52168','52448','52481','56748','56800','58053','59263','62004','62247','129542','67862','69687','71172','71990','72411','76910','77416','77546','77682','77727','78398','79894','80675','80810','80992','82166','83753','85062','86962','92315','92427','92523','92902','95432','95584','95785','97993','100258','100690','102284','105619','106758','107672','108087','109880','110472','111717','112523','112736','113947','113997','115209','122112','124359','14836','125933','127753','128203','132010','133802','124746','133064','702','993','6457','21267','10924','13381','13702','14265','15358','17782','23246','136398','27031','27425','28252','28150','30523','32050','32794','34635','37771','42823','43177','44655','44946','50684','51410','52005','54919','57085','57408','58220','60140','61380','63650','65512','65768','66317','66554','69854','72617','78633','79523','81468','81491','83427','91756','96136','96855','97081','100090','102016','102598','104110','105600','108651','110916','112024','112880','115349','118644','120519','120620','125661','127864','133420','133679','128793','142913','695','1246','2337','2381','5433','6404','9099','12276','12445','15932','16437','18599','18694','19546','23452','24768','24853','25034','27398','29763','30553','30873','31089','32097','33330','35456','36250','38608','39878','39971','43997','44686','46746','48757','49548','51685','53099','55437','56752','57444','60121','60700','61369','62358','62488','65092','66489','68384','70108','71437','72317','73435','73473','73739','77910','79614','79642','79938','81816','85132','86501','125627','92088','94531','96151','97450','97565','98395','98685','99514','100416','102728','103441','104698','104791','106740','110263','114814','117587','118545','121913','122957','124070','44859','124737','125596','127468','129489','131601','132011','132164','132591','133995','491','1399','2081','2862','3644','8115','8243','10811','11263','11424','11719','11796','13725','15619','16293','16539','17174','17205','18091','20814','22654','22827','24036','24600','25372','25896','26193','31569','31609','34670','35309','36605','37242','38197','39556','41210','43805','45478','46290','49485','137039','52305','53306','55623','61885','62154','66046','68178','68628','138866','72758','73840','73874','76640','76899','76986','79001','82142','82154','84763','87844','88049','90041','96272','96322','96382','97760','151361','103104','104357','107505','109315','140742','111571','113776','118599','121132','122174','122645','124115','125147','130751','130878','131980','133071','19139','7261','14110','21560','22495','26053','30648','33822','56583','60119','66404','70003','152800','6606','8501','9780','10791','18497','31565','31907','33368','34016','152742','128863','3339','4710','33487','33792','46435','133428','13178','26532','32979','15772','16282','51793','57564','6748','16936','3677','41404','5822','33857','49341','2304','19946','24390','24511','25682','27128','29635','30854','39651','40001','60083','17282','6692','16854','57771','58654','31013','66104','34221','12254','1699','205556','228564','307','55322','63500','135226','74906','25543','79455','8943','13840','63758','126538','39978','42682','103425','103524','84214','150486','160656','171007','209726','218420','219742','239709','125991','10377','28083','37582','77648','79389','99671','130006','154107','156027','161958','166132','210035','235727','218240','123749','5478','137832','35344','187863','206624','43631','72385','169785','191531','55395','81857','84341','123836','57050','128123','101599','200268','94207','113663','152212','143036','3114','36257','49550','123115','147724','230563','64794','98026','124601','153827','199381','211130'|</t>
+  </si>
+  <si>
+    <t>['142484','116245','142872','43254','1459','134032','143122','15204','155513','181948','142238','191582','185054','208359','113178','192702','236371','190013','6434','231850','128469','172662','222162','122347','158690','202694','56659','85635','3571','83186','227340','41962','217309','52660','161648','184642','3847','2373','62625','65373','58283','58911','237783','79514','110389','144568','5955','78754','96419','83574','223270','148046','191859','33879','52936','106804','221612','61663','207542','213989','49369','116055','151927','8514','100535','187338','207180','50936','11886','20763','230376','134949','151680','152016','164646','206572','178897','181797','183160','206869','187675','200594','222412','223723','233024','234608','235990','240241','203425','186746','215740','227893','230795','147716','150821','151683','155087','173389','208781','221871','236646','134575','138298','141692','146223','147538','148715','154723','155770','159371','166226','166447','185614','190700','200435','203431','209303','211686','225506','226857','231874','236181','134829','153445','188330','195998','215567','236722','240378','136118','144038','145786','156369','160789','166893','177498','184217','197688','212943','223606','224837','225080','228898','229908','234747','236146','236944','139179','140483','141333','141742','149927','150157','153100','157664','160763','164828','165203','166177','167379','169768','170121','170176','171097','172136','172760','174951','176543','188603','188635','192839','194021','194266','196939','199268','207526','207791','209874','210350','216983','219655','221577','225998','231823','233786','139210','139560','140971','148938','153385','156024','156566','157189','161540','162805','165776','181190','183554','184555','185691','187767','192580','196291','200692','203271','205426','209161','212361','212521','214551','220751','221103','222785','226178','234948','236366','238464','140303','155940','171027','184033','193357','206646','228561','240057','158140','159829','168276','181627','181985','194704','199802','200515','214462','220549','224670','231114','231559','238379','239180','139056','146495','160004','163839','170485','174902','176024','181799','188941','190575','192751','195570','212682','215390','222246','227246','232402','233696','238260','238366','138674','140217','149213','151733','155395','156878','157846','182991','197481','200860','204224','212394','215129','151466','157857','205201','208419','222958','224064','238013','142841','145861','145877','146423','165161','166962','171677','197554','199848','218849','219161','221310','234670','235539','239758','136089','138309','139280','139552','139972','140112','141291','145092','146832','147765','148030','149426','151459','151615','153585','154644','155425','156031','162031','158373','161939','163262','164664','168617','169885','169922','171070','173586','177972','178711','179427','179543','181848','183383','186074','186323','186484','186645','188930','189510','194658','197850','198151','204452','208462','210041','210801','211161','213948','214599','217006','220057','222119','229206','229762','236497','237377','240264','139906','142689','144492','161710','171251','173347','182732','199171','199748','218496','157559','161139','162145','175894','177668','179093','191030','211557','217141','218850','140479','152927','154431','154464','159986','179970','179999','184576','180201','187575','189920','190567','192647','207120','208849','212153','214562','218163','229721','229883','230166','233318','235390','135669','136042','146188','146794','150655','155019','159866','160735','164404','165424','172541','186414','176530','178186','181487','185242','190676','193814','196736','206032','212641','224220','224416','225635','233901','234701','237931','138231','141323','144648','145555','150780','150899','152839','156034','156206','157204','163155','164382','164577','166037','167180','171781','172656','175940','176083','176527','177893','179370','179380','180506','180928','181312','186261','186821','188752','188829','192028','192253','195430','196757','197324','204858','202564','203048','209777','209943','211983','215123','215882','217903','219176','227481','232103','234356','239047','144314','152718','161890','173232','184010','185603','189087','192262','195632','202699','223098','223836','224922','229421','140000','140062','168535','175315','179702','193716','211405','226429','212193','229689','156794','159799','163819','179634','181429','190947','205996','211049','224660','134586','140179','140897','148743','148792','153916','155447','161638','161681','163049','163218','186378','169820','177857','178398','182872','183800','188456','191281','191863','194747','199020','201060','205442','210315','214715','217037','218199','228236','229366','230278','230745','238378','238645','141358','141807','146429','151549','163349','159431','163012','176825','178193','189427','189930','191574','194472','196651','199478','205863','225950','231182','146349','161436','187104','191021','191734','194086','197836','203209','230430','136919','147914','150225','151174','151776','166433','170224','177521','185308','192052','200711','206227','210308','222863','222913','231145','236127','137197','140158','146957','148680','158508','167413','181146','188059','195832','215406','219282','221742','228771','230227','233235','137687','139905','148683','153540','154931','160185','161507','168943','175576','190299','194794','211649','213228','218327','227520','137733','143531','145229','152035','156082','162358','162560','166563','167482','174906','177785','179581','181727','184831','187591','188181','192875','197918','203955','205171','206049','211102','211511','140460','182042','185846','186059','194978','202325','207738','210823','213539','224910','143750','146664','157155','171037','185610','214994','222640','236462','135958','145554','152220','154793','155394','157781','173632','179192','190668','186750','191225','206920','218691','219325','221114','135888','137520','140523','142060','144519','145787','146424','147199','147684','154270','160406','161101','161838','163303','163875','164094','164561','166429','168479','168736','169732','172313','172383','175207','176225','178036','182775','186511','187648','188736','190841','194156','195367','195774','204083','210774','212113','214198','216378','218821','220433','232024','232440','235333','236582','239376','200511','200703','216368','216854','220985','221684','221834','221849','222135','223137','223721','224158','224504','226166','226297','226695','229251','230716','230761','234635','234895','235308','236196','237124','237960','238930','239976','240032','122105','168573','96922','144185','151931','156986','190213','217362','164013','104780','121861','167901','184630','124937','185146','193248','195079','77300','80971','86658','131929','204467','143637','203758','81361','106807','80313','131985','159184','212516','219061','143680','199109','200379','210667','213357','88336','90589','160050','187722','190416','196196','216274','108357','158067','191814','209748','218028','168409','88808','91652','107419','120394','130934','176535','186299','215284','72338','150378','155290','156516','157947','216010','219839','96387','103082','120734','122770','146527','147644','184966','107876','175298','184668','149130','150004','156304','174164','189171','84614','88533','90706','156563','179208','199464','80947','84283','85985','96257','101054','108605','122529','133615','137288','152785','169737','172060','218831','219358','83489','92916','108429','117211','119645','150610','149445','170454','184703','189645','190838','191674','214057','92414','115798','119426','128986','140277','154095','155957','160911','181632','126037','142972','305','557','784','3098','3672','4208','6537','7626','8122','9776','13779','16415','17391','17442','17741','18019','18138','20033','22734','23111','25358','26767','27364','27864','29168','30409','34851','35629','40383','37821','37934','38939','41644','42197','42305','42734','43507','43919','44444','44863','47006','47204','48052','59307','50573','53776','57248','58083','58533','62498','64663','65211','65916','66016','66723','67740','70467','73642','77256','78947','78958','79333','80104','80443','80717','81835','82425','82968','84578','87717','91015','91765','93806','96354','99101','99674','99978','103749','103853','104550','104801','105053','105736','105868','110303','110562','111378','111785','114642','117175','118705','123784','127336','127500','128766','129848','132134','132751','132950','133166','133776','131234','3671','4081','135435','12530','14875','25798','27308','30244','36571','41743','43437','44422','50607','55895','60525','66798','68600','68660','80402','82849','84693','92321','96066','107805','113252','116607','124001','130014','133034','132020','133819','1614','9787','15251','16859','18125','18253','21029','22044','24430','25821','30558','35912','39172','43686','44759','48274','48348','48952','49643','52210','55580','56230','56407','57930','57995','63830','65413','138646','71351','77608','102025','83878','84727','85039','89242','90596','91378','93895','94043','100388','101217','105518','106584','108694','111679','115046','114720','115805','118622','118763','119139','124080','128823','131551','132161','132761','132835','968','2145','2916','3901','7554','8131','8405','8875','9938','11008','11260','11633','14409','23443','27408','28907','29640','37909','38528','40120','60775','41112','42345','43161','44010','45630','46261','48335','54169','56205','57845','62892','65927','71052','72573','72609','72949','74596','74997','76347','77748','77875','78079','78374','79904','80019','80515','80904','81473','84188','102028','85108','92610','96690','98837','102417','103518','106075','106994','107133','107743','108418','109053','111513','114441','152173','120001','120466','124740','127774','129389','131553','133568','142275','128616','132155','124431','1835','4852','5970','5985','6412','6955','7065','7703','8979','9049','9917','10941','11426','13336','15743','15897','16700','17972','19474','21410','22635','23082','27277','29120','30449','31299','36733','37519','37960','38880','39273','43509','46157','46514','46973','50361','51850','53952','54531','57203','58449','62391','62627','62868','63596','138384','65272','67241','68865','69075','72535','73049','74789','75400','77048','79462','81655','86241','88606','88789','89145','89600','92602','94657','94900','95113','102086','95695','96505','100305','100408','100617','100621','100751','103105','105168','105373','105472','106890','110314','110661','111108','111294','112819','113515','117619','119304','120316','120521','120528','120659','124907','126403','129765','131946','132840','153878','5','803','2639','5453','5594','129144','8608','8891','11318','12098','12783','17960','18400','18679','20839','23247','23479','23920','25659','26382','28634','31791','33691','36559','37647','37686','38127','38824','38946','40172','43126','44441','45829','46984','47544','49109','49486','52170','128455','57399','58303','63100','63763','64448','64981','65895','128047','66289','67269','67319','69236','70023','71428','71681','74427','75660','75870','76389','77814','78152','81308','80554','127991','82858','83539','84011','88645','89138','89758','92226','94088','95964','97567','98652','100307','101113','102703','104239','105170','106108','106842','106907','109530','110458','114806','114884','114941','115031','116830','118122','120000','121285','9024','128624','129618','130084','132992','2029','2594','3371','6931','7325','8446','8837','10917','12757','13544','14020','17641','17956','19344','21647','22075','39354','24708','24967','29565','29572','30608','31214','32653','33914','34278','36147','38435','41529','44877','47239','48848','48908','51292','52433','52552','52699','52792','54130','56588','57681','58385','58941','59934','127472','60452','127483','65780','66892','67721','69590','69747','69880','70898','72508','74337','78317','79008','81699','82051','82348','83068','84196','86674','89038','90018','91299','92325','125673','93518','125382','98274','125485','99009','101785','102137','103741','104396','105700','108474','110143','110357','111635','111934','114266','114681','114932','115534','115558','115652','117848','118484','119292','119814','120456','120690','120792','120862','122837','135325','127676','130746','131123','128759','147482','410','5228','5975','6468','8136','13556','16203','20203','20467','21150','21907','22013','26278','27384','28663','30270','31941','32840','34162','34185','36119','36564','37307','39104','40441','40582','40730','42225','43182','165199','44991','45563','47205','47802','47968','48521','49230','50162','50277','50444','51280','52168','52448','52481','56748','56800','58053','59263','62004','62247','129542','67862','69687','71172','71990','72411','76910','77416','77546','77682','77727','78398','79894','80675','80810','80992','82166','83753','85062','86962','92315','92427','92523','92902','95432','95584','95785','97993','100258','100690','102284','105619','106758','107672','108087','109880','110472','111717','112523','112736','113947','113997','115209','122112','124359','14836','125933','127753','128203','132010','133802','124746','133064','702','993','6457','21267','10924','13381','13702','14265','15358','17782','23246','136398','27031','27425','28252','28150','30523','32050','32794','34635','37771','42823','43177','44655','44946','50684','51410','52005','54919','57085','57408','58220','60140','61380','63650','65512','65768','66317','66554','69854','72617','78633','79523','81468','81491','83427','91756','96136','96855','97081','100090','102016','102598','104110','105600','108651','110916','112024','112880','115349','118644','120519','120620','125661','127864','133420','133679','128793','142913','695','1246','2337','2381','5433','6404','9099','12276','12445','15932','16437','18599','18694','19546','23452','24768','24853','25034','27398','29763','30553','30873','31089','32097','33330','35456','36250','38608','39878','39971','43997','44686','46746','48757','49548','51685','53099','55437','56752','57444','60121','60700','61369','62358','62488','65092','66489','68384','70108','71437','72317','73435','73473','73739','77910','79614','79642','79938','81816','85132','86501','125627','92088','94531','96151','97450','97565','98395','98685','99514','100416','102728','103441','104698','104791','106740','110263','114814','117587','118545','121913','122957','124070','44859','124737','125596','127468','129489','131601','132011','132164','132591','133995','491','1399','2081','2862','3644','8115','8243','10811','11263','11424','11719','11796','13725','15619','16293','16539','17174','17205','18091','20814','22654','22827','24036','24600','25372','25896','26193','31569','31609','34670','35309','36605','37242','38197','39556','41210','43805','45478','46290','49485','137039','52305','53306','55623','61885','62154','66046','68178','68628','138866','72758','73840','73874','76640','76899','76986','79001','82142','82154','84763','87844','88049','90041','96272','96322','96382','97760','151361','103104','104357','107505','109315','140742','111571','113776','118599','121132','122174','122645','124115','125147','130751','130878','131980','133071','19139','7261','14110','21560','22495','26053','30648','33822','56583','60119','66404','70003','152800','6606','8501','9780','10791','18497','31565','31907','33368','34016','152742','128863','3339','4710','33487','33792','46435','133428','13178','26532','32979','15772','16282','51793','57564','6748','16936','3677','41404','5822','33857','49341','2304','19946','24390','24511','25682','27128','29635','30854','39651','40001','60083','17282','6692','16854','57771','58654','31013','66104','34221','12254','1699','205556','228564','307','55322','63500','135226','74906','25543','79455','8943','13840','63758','126538','39978','42682','103425','103524','84214','150486','160656','171007','209726','218420','219742','239709','125991','10377','28083','37582','77648','79389','99671','130006','154107','156027','161958','166132','210035','235727','218240','123749','5478','137832','35344','187863','206624','43631','72385','169785','191531','55395','81857','84341','123836','57050','128123','101599','200268','94207','113663','152212','143036','3114','36257','49550','123115','147724','230563','64794','98026','124601','153827','199381','211130']</t>
+  </si>
+  <si>
+    <t>[0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056]</t>
   </si>
 </sst>
 </file>
@@ -5885,8 +5885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6197,14 +6197,14 @@
       </c>
       <c r="B26" s="18">
         <f>IF(D26&lt;&gt;"",D26,IF(LEN(INDEX(Lookups!$C$19:$AF$28,2,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)-1))=0,"",INDEX(Lookups!$C$19:$AF$28,2,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)-1)))</f>
-        <v>6</v>
+        <v>1921</v>
       </c>
       <c r="C26" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$19:$AF$28,2,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)))=0,"",INDEX(Lookups!$C$19:$AF$28,2,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
       <c r="D26" s="27">
-        <v>6</v>
+        <v>1921</v>
       </c>
       <c r="E26" s="23"/>
     </row>
@@ -6468,13 +6468,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="23" t="s">
+        <v>747</v>
+      </c>
+      <c r="B46" s="18" t="s">
         <v>748</v>
       </c>
-      <c r="B46" s="18" t="s">
+      <c r="C46" s="23" t="s">
         <v>749</v>
-      </c>
-      <c r="C46" s="23" t="s">
-        <v>750</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -6552,8 +6552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6788,7 +6788,7 @@
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
@@ -6826,31 +6826,31 @@
       </c>
       <c r="H6" s="42"/>
       <c r="I6" s="45" t="s">
+        <v>750</v>
+      </c>
+      <c r="J6" s="42" t="s">
         <v>752</v>
       </c>
-      <c r="J6" s="42" t="s">
+      <c r="K6" s="43">
+        <v>0</v>
+      </c>
+      <c r="L6" s="43">
+        <v>0</v>
+      </c>
+      <c r="M6" s="43">
+        <v>0</v>
+      </c>
+      <c r="N6" s="43">
+        <v>0</v>
+      </c>
+      <c r="O6" s="43">
+        <v>0</v>
+      </c>
+      <c r="P6" s="43" t="s">
         <v>753</v>
       </c>
-      <c r="K6" s="43">
-        <v>0</v>
-      </c>
-      <c r="L6" s="43">
-        <v>0</v>
-      </c>
-      <c r="M6" s="43">
-        <v>0</v>
-      </c>
-      <c r="N6" s="43">
-        <v>0</v>
-      </c>
-      <c r="O6" s="43">
-        <v>0</v>
-      </c>
-      <c r="P6" s="43" t="s">
-        <v>751</v>
-      </c>
       <c r="Q6" s="43" t="s">
-        <v>747</v>
+        <v>754</v>
       </c>
       <c r="R6" s="42" t="s">
         <v>746</v>

</xml_diff>

<commit_message>
Updating measure to add nearby buildings as shading
</commit_message>
<xml_diff>
--- a/spreadsheet/urban-spreadsheet.xlsx
+++ b/spreadsheet/urban-spreadsheet.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2194" uniqueCount="755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2128" uniqueCount="720">
   <si>
     <t>type</t>
   </si>
@@ -1926,24 +1926,6 @@
     <t>integer</t>
   </si>
   <si>
-    <t>Total Natural Gas Intensity</t>
-  </si>
-  <si>
-    <t>total_natural_gas_intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.total_natural_gas</t>
-  </si>
-  <si>
-    <t>Total Electricity Intensity</t>
-  </si>
-  <si>
-    <t>total_electricity_intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.total_electricity</t>
-  </si>
-  <si>
     <t>Parameter Short Display Name</t>
   </si>
   <si>
@@ -2016,105 +1998,6 @@
     <t>m2</t>
   </si>
   <si>
-    <t>Natural Gas Heating Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.heating_natural_gas</t>
-  </si>
-  <si>
-    <t>Cooling Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.cooling_electricity</t>
-  </si>
-  <si>
-    <t>Interior Lighting Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.interior_lighting_electricity</t>
-  </si>
-  <si>
-    <t>Exterior Lighting Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.exterior_lighting_electricity</t>
-  </si>
-  <si>
-    <t>Equipment Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.interior_equipment_electricity</t>
-  </si>
-  <si>
-    <t>Equipment Natural Gas Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.interior_equipment_natural_gas</t>
-  </si>
-  <si>
-    <t>Experior Equipment Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.exterior_equipment_electricity</t>
-  </si>
-  <si>
-    <t>Fans Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.fans_electricity</t>
-  </si>
-  <si>
-    <t>Pumps Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.pumps_electricity</t>
-  </si>
-  <si>
-    <t>Heat Rejection Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.heat_rejection_electricity</t>
-  </si>
-  <si>
-    <t>Humidification Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.humidification_electricity</t>
-  </si>
-  <si>
-    <t>Water Systems Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.water_systems_electricity</t>
-  </si>
-  <si>
-    <t>Water Systems Natural Gas Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.water_systems_natural_gas</t>
-  </si>
-  <si>
-    <t>Refrigeration Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.refrigeration_electricity</t>
-  </si>
-  <si>
-    <t>Total Life Cycle Cost</t>
-  </si>
-  <si>
-    <t>standard_report.total_life_cycle_cost</t>
-  </si>
-  <si>
-    <t>$</t>
-  </si>
-  <si>
-    <t>NG EUI</t>
-  </si>
-  <si>
-    <t>Elec EUI</t>
-  </si>
-  <si>
     <t>standard_reports.time_setpoint_not_met_during_occupied_cooling</t>
   </si>
   <si>
@@ -2305,6 +2188,18 @@
   </si>
   <si>
     <t>[0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056]</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.total_energy</t>
+  </si>
+  <si>
+    <t>Total Energy</t>
+  </si>
+  <si>
+    <t>total_energy_intensity</t>
+  </si>
+  <si>
+    <t>EUI</t>
   </si>
 </sst>
 </file>
@@ -5885,8 +5780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5924,7 +5819,7 @@
         <v>435</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>710</v>
+        <v>671</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>436</v>
@@ -5935,7 +5830,7 @@
         <v>457</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>726</v>
+        <v>687</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>458</v>
@@ -5946,7 +5841,7 @@
         <v>470</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>733</v>
+        <v>694</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>611</v>
@@ -5957,7 +5852,7 @@
         <v>471</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>727</v>
+        <v>688</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>473</v>
@@ -6018,28 +5913,28 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="24" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="E9" s="24" t="str">
         <f>"$"&amp;VALUE(LEFT(E7,5))+B9*VALUE(LEFT(E8,5))&amp;"/hour"</f>
         <v>$1.96/hour</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>708</v>
+        <v>669</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
-        <v>698</v>
+        <v>659</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>699</v>
+        <v>660</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
       <c r="F10" s="2" t="s">
-        <v>700</v>
+        <v>661</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -6057,7 +5952,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>745</v>
+        <v>706</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>472</v>
@@ -6068,7 +5963,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>734</v>
+        <v>695</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>612</v>
@@ -6104,7 +5999,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>709</v>
+        <v>670</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -6412,7 +6307,7 @@
         <v>28</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>735</v>
+        <v>696</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -6438,13 +6333,13 @@
         <v>31</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>695</v>
+        <v>656</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>40</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>736</v>
+        <v>697</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>449</v>
@@ -6468,29 +6363,29 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="23" t="s">
-        <v>747</v>
+        <v>708</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>748</v>
+        <v>709</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>749</v>
+        <v>710</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>701</v>
+        <v>662</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>702</v>
+        <v>663</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>703</v>
+        <v>664</v>
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="19"/>
       <c r="F48" s="8" t="s">
-        <v>704</v>
+        <v>665</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -6505,18 +6400,18 @@
     </row>
     <row r="51" spans="1:6" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
-        <v>705</v>
+        <v>666</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>706</v>
+        <v>667</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>703</v>
+        <v>664</v>
       </c>
       <c r="D51" s="19"/>
       <c r="E51" s="19"/>
       <c r="F51" s="8" t="s">
-        <v>707</v>
+        <v>668</v>
       </c>
     </row>
   </sheetData>
@@ -6553,7 +6448,7 @@
   <dimension ref="A1:Z56"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6671,7 +6566,7 @@
         <v>35</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="G3" s="37" t="s">
         <v>11</v>
@@ -6737,13 +6632,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>737</v>
+        <v>698</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>743</v>
+        <v>704</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>737</v>
+        <v>698</v>
       </c>
       <c r="E4" s="39" t="s">
         <v>67</v>
@@ -6777,10 +6672,10 @@
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>739</v>
+        <v>700</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>738</v>
+        <v>699</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15" t="s">
@@ -6788,7 +6683,7 @@
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15" t="s">
-        <v>751</v>
+        <v>712</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
@@ -6815,10 +6710,10 @@
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42" t="s">
-        <v>741</v>
+        <v>702</v>
       </c>
       <c r="E6" s="42" t="s">
-        <v>740</v>
+        <v>701</v>
       </c>
       <c r="F6" s="42"/>
       <c r="G6" s="42" t="s">
@@ -6826,10 +6721,10 @@
       </c>
       <c r="H6" s="42"/>
       <c r="I6" s="45" t="s">
-        <v>750</v>
+        <v>711</v>
       </c>
       <c r="J6" s="42" t="s">
-        <v>752</v>
+        <v>713</v>
       </c>
       <c r="K6" s="43">
         <v>0</v>
@@ -6847,13 +6742,13 @@
         <v>0</v>
       </c>
       <c r="P6" s="43" t="s">
-        <v>753</v>
+        <v>714</v>
       </c>
       <c r="Q6" s="43" t="s">
-        <v>754</v>
+        <v>715</v>
       </c>
       <c r="R6" s="42" t="s">
-        <v>746</v>
+        <v>707</v>
       </c>
       <c r="S6" s="42"/>
       <c r="T6" s="42"/>
@@ -6869,13 +6764,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>742</v>
+        <v>703</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>744</v>
+        <v>705</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>742</v>
+        <v>703</v>
       </c>
       <c r="E7" s="39" t="s">
         <v>67</v>
@@ -8291,11 +8186,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M94"/>
+  <dimension ref="A1:M92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8338,7 +8233,7 @@
         <v>460</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="C2" s="35" t="s">
         <v>615</v>
@@ -8377,7 +8272,7 @@
         <v>622</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="C3" s="35" t="s">
         <v>623</v>
@@ -8411,87 +8306,73 @@
     </row>
     <row r="4" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>628</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>689</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>629</v>
-      </c>
+        <v>646</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
-        <v>630</v>
+        <v>652</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>469</v>
+        <v>647</v>
       </c>
       <c r="F4" s="15" t="s">
         <v>63</v>
       </c>
       <c r="G4" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="15" t="b">
         <v>1</v>
       </c>
       <c r="I4" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="15">
-        <v>140</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J4" s="15"/>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
     </row>
     <row r="5" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>631</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>690</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>632</v>
-      </c>
+        <v>648</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>633</v>
+        <v>653</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>469</v>
+        <v>647</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>63</v>
       </c>
       <c r="G5" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="15" t="b">
         <v>1</v>
       </c>
       <c r="I5" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="15">
-        <v>590</v>
-      </c>
-      <c r="K5" s="15">
-        <v>5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
     </row>
     <row r="6" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>691</v>
+        <v>654</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="F6" s="15" t="s">
         <v>63</v>
@@ -8512,15 +8393,15 @@
     </row>
     <row r="7" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>692</v>
+        <v>655</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>63</v>
@@ -8541,492 +8422,274 @@
     </row>
     <row r="8" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>655</v>
-      </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
+        <v>717</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>719</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>718</v>
+      </c>
       <c r="D8" s="15" t="s">
-        <v>693</v>
+        <v>716</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>653</v>
+        <v>469</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>63</v>
       </c>
       <c r="G8" s="15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="15" t="b">
         <v>1</v>
       </c>
       <c r="I8" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="15"/>
+        <v>1</v>
+      </c>
+      <c r="J8" s="15">
+        <v>0</v>
+      </c>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
     </row>
     <row r="9" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
-        <v>656</v>
-      </c>
+      <c r="A9" s="15"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
-      <c r="D9" s="15" t="s">
-        <v>694</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>657</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I9" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
     </row>
     <row r="10" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
-        <v>658</v>
-      </c>
+      <c r="A10" s="15"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
-      <c r="D10" s="15" t="s">
-        <v>659</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
     </row>
     <row r="11" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>660</v>
-      </c>
+      <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
-      <c r="D11" s="15" t="s">
-        <v>661</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
     </row>
     <row r="12" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
-        <v>662</v>
-      </c>
+      <c r="A12" s="15"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
-      <c r="D12" s="15" t="s">
-        <v>663</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
     </row>
-    <row r="13" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
-        <v>664</v>
-      </c>
+    <row r="13" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
-      <c r="D13" s="15" t="s">
-        <v>665</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
     </row>
-    <row r="14" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>666</v>
-      </c>
+    <row r="14" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
-      <c r="D14" s="15" t="s">
-        <v>667</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
     </row>
     <row r="15" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>668</v>
-      </c>
+      <c r="A15" s="15"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
-      <c r="D15" s="15" t="s">
-        <v>669</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I15" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
     </row>
     <row r="16" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
-        <v>670</v>
-      </c>
+      <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
-      <c r="D16" s="15" t="s">
-        <v>671</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I16" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
     </row>
     <row r="17" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
-        <v>672</v>
-      </c>
+      <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
-      <c r="D17" s="15" t="s">
-        <v>673</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
     </row>
     <row r="18" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
-        <v>674</v>
-      </c>
+      <c r="A18" s="15"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
-      <c r="D18" s="15" t="s">
-        <v>675</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
     </row>
-    <row r="19" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
-        <v>676</v>
-      </c>
+    <row r="19" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
-      <c r="D19" s="15" t="s">
-        <v>677</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
     </row>
-    <row r="20" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
-        <v>678</v>
-      </c>
+    <row r="20" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
-      <c r="D20" s="15" t="s">
-        <v>679</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
     </row>
     <row r="21" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
-        <v>680</v>
-      </c>
+      <c r="A21" s="15"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
-      <c r="D21" s="15" t="s">
-        <v>681</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
     </row>
     <row r="22" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>682</v>
-      </c>
+      <c r="A22" s="15"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
-      <c r="D22" s="15" t="s">
-        <v>683</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I22" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
       <c r="M22" s="15"/>
     </row>
-    <row r="23" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
-        <v>684</v>
-      </c>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="15"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
-      <c r="D23" s="15" t="s">
-        <v>685</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I23" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
     </row>
-    <row r="24" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
-        <v>686</v>
-      </c>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
-      <c r="D24" s="15" t="s">
-        <v>687</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>688</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G24" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I24" s="15" t="b">
-        <v>0</v>
-      </c>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
@@ -9063,34 +8726,10 @@
       <c r="M26" s="15"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
+      <c r="B27" s="22"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
+      <c r="B28" s="22"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B29" s="22"/>
@@ -9283,12 +8922,6 @@
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92" s="22"/>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B93" s="22"/>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B94" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -17500,7 +17133,7 @@
         <v>438</v>
       </c>
       <c r="D1" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -17508,19 +17141,19 @@
     </row>
     <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -17534,10 +17167,10 @@
         <v>591</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -17551,10 +17184,10 @@
         <v>593</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -17568,10 +17201,10 @@
         <v>595</v>
       </c>
       <c r="D5" s="22" t="s">
+        <v>637</v>
+      </c>
+      <c r="E5" s="22" t="s">
         <v>643</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -17585,10 +17218,10 @@
         <v>597</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>696</v>
+        <v>657</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -17602,10 +17235,10 @@
         <v>599</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>696</v>
+        <v>657</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -17619,10 +17252,10 @@
         <v>600</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>697</v>
+        <v>658</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -17636,10 +17269,10 @@
         <v>602</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>697</v>
+        <v>658</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -17647,16 +17280,16 @@
         <v>603</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>604</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>697</v>
+        <v>658</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -17724,18 +17357,18 @@
         <v>553</v>
       </c>
       <c r="U18" s="22" t="s">
-        <v>716</v>
+        <v>677</v>
       </c>
       <c r="V18" s="22"/>
       <c r="W18" s="22"/>
       <c r="X18" t="s">
-        <v>711</v>
+        <v>672</v>
       </c>
       <c r="AA18" t="s">
-        <v>712</v>
+        <v>673</v>
       </c>
       <c r="AD18" s="22" t="s">
-        <v>728</v>
+        <v>689</v>
       </c>
       <c r="AE18" s="22"/>
       <c r="AF18" s="22"/>
@@ -17781,16 +17414,16 @@
         <v>580</v>
       </c>
       <c r="U19" s="22" t="s">
-        <v>725</v>
+        <v>686</v>
       </c>
       <c r="V19" s="22" t="s">
-        <v>718</v>
+        <v>679</v>
       </c>
       <c r="W19" s="22" t="s">
-        <v>718</v>
+        <v>679</v>
       </c>
       <c r="AA19" s="22" t="s">
-        <v>713</v>
+        <v>674</v>
       </c>
       <c r="AB19" s="22">
         <v>30</v>
@@ -17799,13 +17432,13 @@
         <v>589</v>
       </c>
       <c r="AD19" s="22" t="s">
-        <v>729</v>
+        <v>690</v>
       </c>
       <c r="AE19" s="22" t="b">
         <v>1</v>
       </c>
       <c r="AF19" s="22" t="s">
-        <v>730</v>
+        <v>691</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.3">
@@ -17855,16 +17488,16 @@
         <v>2</v>
       </c>
       <c r="W20" s="22" t="s">
-        <v>717</v>
+        <v>678</v>
       </c>
       <c r="AD20" s="22" t="s">
-        <v>731</v>
+        <v>692</v>
       </c>
       <c r="AE20" s="22" t="b">
         <v>1</v>
       </c>
       <c r="AF20" s="22" t="s">
-        <v>732</v>
+        <v>693</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.3">
@@ -17942,13 +17575,13 @@
         <v>541</v>
       </c>
       <c r="L23" s="22" t="s">
-        <v>721</v>
+        <v>682</v>
       </c>
       <c r="M23" s="22">
         <v>1</v>
       </c>
       <c r="N23" s="23" t="s">
-        <v>722</v>
+        <v>683</v>
       </c>
       <c r="O23" s="23" t="s">
         <v>568</v>
@@ -17994,16 +17627,16 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>716</v>
+        <v>677</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>714</v>
+        <v>675</v>
       </c>
       <c r="J25" s="23">
         <v>0</v>
       </c>
       <c r="K25" s="23" t="s">
-        <v>715</v>
+        <v>676</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>539</v>
@@ -18015,18 +17648,18 @@
         <v>578</v>
       </c>
       <c r="O25" s="23" t="s">
-        <v>723</v>
+        <v>684</v>
       </c>
       <c r="P25" s="22">
         <v>2</v>
       </c>
       <c r="Q25" s="22" t="s">
-        <v>724</v>
+        <v>685</v>
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>711</v>
+        <v>672</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>544</v>
@@ -18046,7 +17679,7 @@
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>712</v>
+        <v>673</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>558</v>
@@ -18069,7 +17702,7 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
-        <v>728</v>
+        <v>689</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>559</v>
@@ -18081,13 +17714,13 @@
         <v>575</v>
       </c>
       <c r="O28" t="s">
-        <v>714</v>
+        <v>675</v>
       </c>
       <c r="P28" s="23">
         <v>0</v>
       </c>
       <c r="Q28" s="23" t="s">
-        <v>715</v>
+        <v>676</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.3">
@@ -18111,24 +17744,24 @@
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.3">
       <c r="L31" s="22" t="s">
-        <v>714</v>
+        <v>675</v>
       </c>
       <c r="M31" s="23">
         <v>0</v>
       </c>
       <c r="N31" s="23" t="s">
-        <v>715</v>
+        <v>676</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.3">
       <c r="L32" t="s">
-        <v>719</v>
+        <v>680</v>
       </c>
       <c r="M32" s="23">
         <v>1</v>
       </c>
       <c r="N32" s="23" t="s">
-        <v>720</v>
+        <v>681</v>
       </c>
     </row>
   </sheetData>

</xml_diff>